<commit_message>
changes to create extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testDataForTestEnvironment.xlsx
+++ b/src/test/resources/testData/testDataForTestEnvironment.xlsx
@@ -383,10 +383,10 @@
     <t>local_gas_station</t>
   </si>
   <si>
-    <t>Policy_P27022024_</t>
-  </si>
-  <si>
-    <t>Report_P27022024_</t>
+    <t>Policy_P28022024_</t>
+  </si>
+  <si>
+    <t>Report_P28022024_</t>
   </si>
 </sst>
 </file>
@@ -931,7 +931,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
script change for parallel testing
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testDataForTestEnvironment.xlsx
+++ b/src/test/resources/testData/testDataForTestEnvironment.xlsx
@@ -317,76 +317,76 @@
     <t>Browser Name (chrome/firefox/edge)</t>
   </si>
   <si>
+    <t>className_one</t>
+  </si>
+  <si>
+    <t>className_two_class_With_Same_Name</t>
+  </si>
+  <si>
+    <t>className_two_class_With_Different_Name</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>invert_colors</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Offshore</t>
+  </si>
+  <si>
+    <t>class_Name_Offshore_Renewables_With_Entity_Name</t>
+  </si>
+  <si>
+    <t>https://test-eh.ebixexchange.com/login</t>
+  </si>
+  <si>
+    <t>suneel.k</t>
+  </si>
+  <si>
+    <t>ebix@123</t>
+  </si>
+  <si>
+    <t>Property,Property</t>
+  </si>
+  <si>
+    <t>Offshore,Terrorism</t>
+  </si>
+  <si>
+    <t>Offshore (Entity A)</t>
+  </si>
+  <si>
+    <t>user2b</t>
+  </si>
+  <si>
+    <t>Hint (Locator value as per class name)</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>peril_Name</t>
+  </si>
+  <si>
+    <t>OffshoreXL</t>
+  </si>
+  <si>
+    <t>local_gas_station</t>
+  </si>
+  <si>
     <t>chrome</t>
   </si>
   <si>
-    <t>className_one</t>
-  </si>
-  <si>
-    <t>className_two_class_With_Same_Name</t>
-  </si>
-  <si>
-    <t>className_two_class_With_Different_Name</t>
-  </si>
-  <si>
-    <t>home</t>
-  </si>
-  <si>
-    <t>grade</t>
-  </si>
-  <si>
-    <t>invert_colors</t>
-  </si>
-  <si>
-    <t>Property</t>
-  </si>
-  <si>
-    <t>Offshore</t>
-  </si>
-  <si>
-    <t>class_Name_Offshore_Renewables_With_Entity_Name</t>
-  </si>
-  <si>
-    <t>https://test-eh.ebixexchange.com/login</t>
-  </si>
-  <si>
-    <t>suneel.k</t>
-  </si>
-  <si>
-    <t>ebix@123</t>
-  </si>
-  <si>
-    <t>Property,Property</t>
-  </si>
-  <si>
-    <t>Offshore,Terrorism</t>
-  </si>
-  <si>
-    <t>Offshore (Entity A)</t>
-  </si>
-  <si>
-    <t>user2b</t>
-  </si>
-  <si>
-    <t>Hint (Locator value as per class name)</t>
-  </si>
-  <si>
-    <t>Fire</t>
-  </si>
-  <si>
-    <t>peril_Name</t>
-  </si>
-  <si>
-    <t>OffshoreXL</t>
-  </si>
-  <si>
-    <t>local_gas_station</t>
-  </si>
-  <si>
-    <t>Policy_P28022024_</t>
-  </si>
-  <si>
-    <t>Report_P28022024_</t>
+    <t>Policy_PY05032024_</t>
+  </si>
+  <si>
+    <t>Report_PY05032024_</t>
   </si>
 </sst>
 </file>
@@ -834,7 +834,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,7 @@
         <v>94</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
         <v>93</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -903,15 +903,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>2</v>
@@ -931,7 +931,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,47 +1039,47 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>98</v>
-      </c>
       <c r="D1" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>110</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="10"/>
@@ -1117,10 +1117,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -1130,27 +1130,27 @@
         <v>18</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>

</xml_diff>

<commit_message>
setup for azure pipeline
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testDataForTestEnvironment.xlsx
+++ b/src/test/resources/testData/testDataForTestEnvironment.xlsx
@@ -383,10 +383,10 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>Policy_PY05032024_</t>
-  </si>
-  <si>
-    <t>Report_PY05032024_</t>
+    <t>Policy_PY06032024_</t>
+  </si>
+  <si>
+    <t>Report_PY06032024_</t>
   </si>
 </sst>
 </file>
@@ -931,7 +931,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes for parallel testing
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testDataForTestEnvironment.xlsx
+++ b/src/test/resources/testData/testDataForTestEnvironment.xlsx
@@ -383,10 +383,10 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>Policy_PY06032024_</t>
-  </si>
-  <si>
-    <t>Report_PY06032024_</t>
+    <t>Policy_PY15032024_</t>
+  </si>
+  <si>
+    <t>Report_PY15032024_</t>
   </si>
 </sst>
 </file>
@@ -883,7 +883,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +931,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes in base class 2
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testDataForTestEnvironment.xlsx
+++ b/src/test/resources/testData/testDataForTestEnvironment.xlsx
@@ -395,10 +395,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>Policy_M18032024_</t>
-  </si>
-  <si>
-    <t>Report_M18032024_</t>
+    <t>Policy_PY20032024_</t>
+  </si>
+  <si>
+    <t>Report_PY20032024_</t>
   </si>
 </sst>
 </file>

</xml_diff>